<commit_message>
update main, test and transactions.xlsx
</commit_message>
<xml_diff>
--- a/parsePDFs03/Transactions.xlsx
+++ b/parsePDFs03/Transactions.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ojell\Desktop\MyPaMa\_CCs\automate\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ojell\Desktop\Oj\_Automation\parse_pdf-projects\parsePDFs03\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4EBEACB5-F572-46F5-8F82-8CDE8650114C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{189007D4-074C-4F3A-A961-31F2300970DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12480" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{3464B314-3BF4-4D3C-98B0-5BA7420BEEAA}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Sale Date</t>
   </si>
@@ -44,13 +44,19 @@
     <t>Post Date</t>
   </si>
   <si>
-    <t>Transaction Details</t>
-  </si>
-  <si>
     <t>Amount</t>
   </si>
   <si>
     <t>FINANCE CHARGE-RETAIL PURCHASES</t>
+  </si>
+  <si>
+    <t>Transaction</t>
+  </si>
+  <si>
+    <t>Statement Date</t>
+  </si>
+  <si>
+    <t>Due Date</t>
   </si>
 </sst>
 </file>
@@ -423,18 +429,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FF1AF28-C413-4D2C-BC97-D10B67487166}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="4" width="38.7109375" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -442,13 +449,19 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>45368</v>
       </c>
@@ -456,7 +469,7 @@
         <v>45368</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D2">
         <v>381.11</v>

</xml_diff>